<commit_message>
Added UTIL func {i.e create folder} added Plot folder with patient data { e.g table perfusion , ROI, REFF images, REG images} Added ROI MCA Right and ACA TOP
</commit_message>
<xml_diff>
--- a/Matlab_Main/Perfusion_data_Reg_MCA_LEFT.xlsx
+++ b/Matlab_Main/Perfusion_data_Reg_MCA_LEFT.xlsx
@@ -13,7 +13,727 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="1020">
+  <si>
+    <t>set1_1</t>
+  </si>
+  <si>
+    <t>set1_2</t>
+  </si>
+  <si>
+    <t>set2_1</t>
+  </si>
+  <si>
+    <t>set2_2</t>
+  </si>
+  <si>
+    <t>set3_1</t>
+  </si>
+  <si>
+    <t>set3_2</t>
+  </si>
+  <si>
+    <t>set4_1</t>
+  </si>
+  <si>
+    <t>set4_2</t>
+  </si>
+  <si>
+    <t>set5_1</t>
+  </si>
+  <si>
+    <t>set5_2</t>
+  </si>
+  <si>
+    <t>set6_1</t>
+  </si>
+  <si>
+    <t>set6_2</t>
+  </si>
+  <si>
+    <t>set7_1</t>
+  </si>
+  <si>
+    <t>set7_2</t>
+  </si>
+  <si>
+    <t>set8_1</t>
+  </si>
+  <si>
+    <t>set8_2</t>
+  </si>
+  <si>
+    <t>set9_1</t>
+  </si>
+  <si>
+    <t>set9_2</t>
+  </si>
+  <si>
+    <t>set10_1</t>
+  </si>
+  <si>
+    <t>set10_2</t>
+  </si>
+  <si>
+    <t>set11_1</t>
+  </si>
+  <si>
+    <t>set11_2</t>
+  </si>
+  <si>
+    <t>set12_1</t>
+  </si>
+  <si>
+    <t>set12_2</t>
+  </si>
+  <si>
+    <t>set13_1</t>
+  </si>
+  <si>
+    <t>set13_2</t>
+  </si>
+  <si>
+    <t>set14_1</t>
+  </si>
+  <si>
+    <t>set14_2</t>
+  </si>
+  <si>
+    <t>set15_1</t>
+  </si>
+  <si>
+    <t>set15_2</t>
+  </si>
+  <si>
+    <t>set16_1</t>
+  </si>
+  <si>
+    <t>set16_2</t>
+  </si>
+  <si>
+    <t>set17_1</t>
+  </si>
+  <si>
+    <t>set17_2</t>
+  </si>
+  <si>
+    <t>set18_1</t>
+  </si>
+  <si>
+    <t>set18_2</t>
+  </si>
+  <si>
+    <t>set19_1</t>
+  </si>
+  <si>
+    <t>set19_2</t>
+  </si>
+  <si>
+    <t>set20_1</t>
+  </si>
+  <si>
+    <t>set20_2</t>
+  </si>
+  <si>
+    <t>set21_1</t>
+  </si>
+  <si>
+    <t>set21_2</t>
+  </si>
+  <si>
+    <t>set22_1</t>
+  </si>
+  <si>
+    <t>set22_2</t>
+  </si>
+  <si>
+    <t>set23_1</t>
+  </si>
+  <si>
+    <t>set23_2</t>
+  </si>
+  <si>
+    <t>set24_1</t>
+  </si>
+  <si>
+    <t>set24_2</t>
+  </si>
+  <si>
+    <t>set25_1</t>
+  </si>
+  <si>
+    <t>set25_2</t>
+  </si>
+  <si>
+    <t>set26_1</t>
+  </si>
+  <si>
+    <t>set26_2</t>
+  </si>
+  <si>
+    <t>set27_1</t>
+  </si>
+  <si>
+    <t>set27_2</t>
+  </si>
+  <si>
+    <t>set28_1</t>
+  </si>
+  <si>
+    <t>set28_2</t>
+  </si>
+  <si>
+    <t>set29_1</t>
+  </si>
+  <si>
+    <t>set29_2</t>
+  </si>
+  <si>
+    <t>set30_1</t>
+  </si>
+  <si>
+    <t>set30_2</t>
+  </si>
+  <si>
+    <t>set1_1</t>
+  </si>
+  <si>
+    <t>set1_2</t>
+  </si>
+  <si>
+    <t>set2_1</t>
+  </si>
+  <si>
+    <t>set2_2</t>
+  </si>
+  <si>
+    <t>set3_1</t>
+  </si>
+  <si>
+    <t>set3_2</t>
+  </si>
+  <si>
+    <t>set4_1</t>
+  </si>
+  <si>
+    <t>set4_2</t>
+  </si>
+  <si>
+    <t>set5_1</t>
+  </si>
+  <si>
+    <t>set5_2</t>
+  </si>
+  <si>
+    <t>set6_1</t>
+  </si>
+  <si>
+    <t>set6_2</t>
+  </si>
+  <si>
+    <t>set7_1</t>
+  </si>
+  <si>
+    <t>set7_2</t>
+  </si>
+  <si>
+    <t>set8_1</t>
+  </si>
+  <si>
+    <t>set8_2</t>
+  </si>
+  <si>
+    <t>set9_1</t>
+  </si>
+  <si>
+    <t>set9_2</t>
+  </si>
+  <si>
+    <t>set10_1</t>
+  </si>
+  <si>
+    <t>set10_2</t>
+  </si>
+  <si>
+    <t>set11_1</t>
+  </si>
+  <si>
+    <t>set11_2</t>
+  </si>
+  <si>
+    <t>set12_1</t>
+  </si>
+  <si>
+    <t>set12_2</t>
+  </si>
+  <si>
+    <t>set13_1</t>
+  </si>
+  <si>
+    <t>set13_2</t>
+  </si>
+  <si>
+    <t>set14_1</t>
+  </si>
+  <si>
+    <t>set14_2</t>
+  </si>
+  <si>
+    <t>set15_1</t>
+  </si>
+  <si>
+    <t>set15_2</t>
+  </si>
+  <si>
+    <t>set16_1</t>
+  </si>
+  <si>
+    <t>set16_2</t>
+  </si>
+  <si>
+    <t>set17_1</t>
+  </si>
+  <si>
+    <t>set17_2</t>
+  </si>
+  <si>
+    <t>set18_1</t>
+  </si>
+  <si>
+    <t>set18_2</t>
+  </si>
+  <si>
+    <t>set19_1</t>
+  </si>
+  <si>
+    <t>set19_2</t>
+  </si>
+  <si>
+    <t>set20_1</t>
+  </si>
+  <si>
+    <t>set20_2</t>
+  </si>
+  <si>
+    <t>set21_1</t>
+  </si>
+  <si>
+    <t>set21_2</t>
+  </si>
+  <si>
+    <t>set22_1</t>
+  </si>
+  <si>
+    <t>set22_2</t>
+  </si>
+  <si>
+    <t>set23_1</t>
+  </si>
+  <si>
+    <t>set23_2</t>
+  </si>
+  <si>
+    <t>set24_1</t>
+  </si>
+  <si>
+    <t>set24_2</t>
+  </si>
+  <si>
+    <t>set25_1</t>
+  </si>
+  <si>
+    <t>set25_2</t>
+  </si>
+  <si>
+    <t>set26_1</t>
+  </si>
+  <si>
+    <t>set26_2</t>
+  </si>
+  <si>
+    <t>set27_1</t>
+  </si>
+  <si>
+    <t>set27_2</t>
+  </si>
+  <si>
+    <t>set28_1</t>
+  </si>
+  <si>
+    <t>set28_2</t>
+  </si>
+  <si>
+    <t>set29_1</t>
+  </si>
+  <si>
+    <t>set29_2</t>
+  </si>
+  <si>
+    <t>set30_1</t>
+  </si>
+  <si>
+    <t>set30_2</t>
+  </si>
+  <si>
+    <t>set1_1</t>
+  </si>
+  <si>
+    <t>set1_2</t>
+  </si>
+  <si>
+    <t>set2_1</t>
+  </si>
+  <si>
+    <t>set2_2</t>
+  </si>
+  <si>
+    <t>set3_1</t>
+  </si>
+  <si>
+    <t>set3_2</t>
+  </si>
+  <si>
+    <t>set4_1</t>
+  </si>
+  <si>
+    <t>set4_2</t>
+  </si>
+  <si>
+    <t>set5_1</t>
+  </si>
+  <si>
+    <t>set5_2</t>
+  </si>
+  <si>
+    <t>set6_1</t>
+  </si>
+  <si>
+    <t>set6_2</t>
+  </si>
+  <si>
+    <t>set7_1</t>
+  </si>
+  <si>
+    <t>set7_2</t>
+  </si>
+  <si>
+    <t>set8_1</t>
+  </si>
+  <si>
+    <t>set8_2</t>
+  </si>
+  <si>
+    <t>set9_1</t>
+  </si>
+  <si>
+    <t>set9_2</t>
+  </si>
+  <si>
+    <t>set10_1</t>
+  </si>
+  <si>
+    <t>set10_2</t>
+  </si>
+  <si>
+    <t>set11_1</t>
+  </si>
+  <si>
+    <t>set11_2</t>
+  </si>
+  <si>
+    <t>set12_1</t>
+  </si>
+  <si>
+    <t>set12_2</t>
+  </si>
+  <si>
+    <t>set13_1</t>
+  </si>
+  <si>
+    <t>set13_2</t>
+  </si>
+  <si>
+    <t>set14_1</t>
+  </si>
+  <si>
+    <t>set14_2</t>
+  </si>
+  <si>
+    <t>set15_1</t>
+  </si>
+  <si>
+    <t>set15_2</t>
+  </si>
+  <si>
+    <t>set16_1</t>
+  </si>
+  <si>
+    <t>set16_2</t>
+  </si>
+  <si>
+    <t>set17_1</t>
+  </si>
+  <si>
+    <t>set17_2</t>
+  </si>
+  <si>
+    <t>set18_1</t>
+  </si>
+  <si>
+    <t>set18_2</t>
+  </si>
+  <si>
+    <t>set19_1</t>
+  </si>
+  <si>
+    <t>set19_2</t>
+  </si>
+  <si>
+    <t>set20_1</t>
+  </si>
+  <si>
+    <t>set20_2</t>
+  </si>
+  <si>
+    <t>set21_1</t>
+  </si>
+  <si>
+    <t>set21_2</t>
+  </si>
+  <si>
+    <t>set22_1</t>
+  </si>
+  <si>
+    <t>set22_2</t>
+  </si>
+  <si>
+    <t>set23_1</t>
+  </si>
+  <si>
+    <t>set23_2</t>
+  </si>
+  <si>
+    <t>set24_1</t>
+  </si>
+  <si>
+    <t>set24_2</t>
+  </si>
+  <si>
+    <t>set25_1</t>
+  </si>
+  <si>
+    <t>set25_2</t>
+  </si>
+  <si>
+    <t>set26_1</t>
+  </si>
+  <si>
+    <t>set26_2</t>
+  </si>
+  <si>
+    <t>set27_1</t>
+  </si>
+  <si>
+    <t>set27_2</t>
+  </si>
+  <si>
+    <t>set28_1</t>
+  </si>
+  <si>
+    <t>set28_2</t>
+  </si>
+  <si>
+    <t>set29_1</t>
+  </si>
+  <si>
+    <t>set29_2</t>
+  </si>
+  <si>
+    <t>set30_1</t>
+  </si>
+  <si>
+    <t>set30_2</t>
+  </si>
+  <si>
+    <t>set1_1</t>
+  </si>
+  <si>
+    <t>set1_2</t>
+  </si>
+  <si>
+    <t>set2_1</t>
+  </si>
+  <si>
+    <t>set2_2</t>
+  </si>
+  <si>
+    <t>set3_1</t>
+  </si>
+  <si>
+    <t>set3_2</t>
+  </si>
+  <si>
+    <t>set4_1</t>
+  </si>
+  <si>
+    <t>set4_2</t>
+  </si>
+  <si>
+    <t>set5_1</t>
+  </si>
+  <si>
+    <t>set5_2</t>
+  </si>
+  <si>
+    <t>set6_1</t>
+  </si>
+  <si>
+    <t>set6_2</t>
+  </si>
+  <si>
+    <t>set7_1</t>
+  </si>
+  <si>
+    <t>set7_2</t>
+  </si>
+  <si>
+    <t>set8_1</t>
+  </si>
+  <si>
+    <t>set8_2</t>
+  </si>
+  <si>
+    <t>set9_1</t>
+  </si>
+  <si>
+    <t>set9_2</t>
+  </si>
+  <si>
+    <t>set10_1</t>
+  </si>
+  <si>
+    <t>set10_2</t>
+  </si>
+  <si>
+    <t>set11_1</t>
+  </si>
+  <si>
+    <t>set11_2</t>
+  </si>
+  <si>
+    <t>set12_1</t>
+  </si>
+  <si>
+    <t>set12_2</t>
+  </si>
+  <si>
+    <t>set13_1</t>
+  </si>
+  <si>
+    <t>set13_2</t>
+  </si>
+  <si>
+    <t>set14_1</t>
+  </si>
+  <si>
+    <t>set14_2</t>
+  </si>
+  <si>
+    <t>set15_1</t>
+  </si>
+  <si>
+    <t>set15_2</t>
+  </si>
+  <si>
+    <t>set16_1</t>
+  </si>
+  <si>
+    <t>set16_2</t>
+  </si>
+  <si>
+    <t>set17_1</t>
+  </si>
+  <si>
+    <t>set17_2</t>
+  </si>
+  <si>
+    <t>set18_1</t>
+  </si>
+  <si>
+    <t>set18_2</t>
+  </si>
+  <si>
+    <t>set19_1</t>
+  </si>
+  <si>
+    <t>set19_2</t>
+  </si>
+  <si>
+    <t>set20_1</t>
+  </si>
+  <si>
+    <t>set20_2</t>
+  </si>
+  <si>
+    <t>set21_1</t>
+  </si>
+  <si>
+    <t>set21_2</t>
+  </si>
+  <si>
+    <t>set22_1</t>
+  </si>
+  <si>
+    <t>set22_2</t>
+  </si>
+  <si>
+    <t>set23_1</t>
+  </si>
+  <si>
+    <t>set23_2</t>
+  </si>
+  <si>
+    <t>set24_1</t>
+  </si>
+  <si>
+    <t>set24_2</t>
+  </si>
+  <si>
+    <t>set25_1</t>
+  </si>
+  <si>
+    <t>set25_2</t>
+  </si>
+  <si>
+    <t>set26_1</t>
+  </si>
+  <si>
+    <t>set26_2</t>
+  </si>
+  <si>
+    <t>set27_1</t>
+  </si>
+  <si>
+    <t>set27_2</t>
+  </si>
+  <si>
+    <t>set28_1</t>
+  </si>
+  <si>
+    <t>set28_2</t>
+  </si>
+  <si>
+    <t>set29_1</t>
+  </si>
+  <si>
+    <t>set29_2</t>
+  </si>
+  <si>
+    <t>set30_1</t>
+  </si>
+  <si>
+    <t>set30_2</t>
+  </si>
   <si>
     <t>set1_1</t>
   </si>
@@ -2465,184 +3185,184 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>720</v>
+        <v>960</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>721</v>
+        <v>961</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>722</v>
+        <v>962</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>723</v>
+        <v>963</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>724</v>
+        <v>964</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>725</v>
+        <v>965</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>726</v>
+        <v>966</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>727</v>
+        <v>967</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>728</v>
+        <v>968</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>729</v>
+        <v>969</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>730</v>
+        <v>970</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>731</v>
+        <v>971</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>732</v>
+        <v>972</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>733</v>
+        <v>973</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>734</v>
+        <v>974</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>735</v>
+        <v>975</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>736</v>
+        <v>976</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>737</v>
+        <v>977</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>738</v>
+        <v>978</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>739</v>
+        <v>979</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>740</v>
+        <v>980</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>741</v>
+        <v>981</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>742</v>
+        <v>982</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>743</v>
+        <v>983</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>744</v>
+        <v>984</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>745</v>
+        <v>985</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>746</v>
+        <v>986</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>747</v>
+        <v>987</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>748</v>
+        <v>988</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>749</v>
+        <v>989</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>750</v>
+        <v>990</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>751</v>
+        <v>991</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>752</v>
+        <v>992</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>753</v>
+        <v>993</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>754</v>
+        <v>994</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>755</v>
+        <v>995</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>756</v>
+        <v>996</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>757</v>
+        <v>997</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>758</v>
+        <v>998</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>759</v>
+        <v>999</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>760</v>
+        <v>1000</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>761</v>
+        <v>1001</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>762</v>
+        <v>1002</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>763</v>
+        <v>1003</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>764</v>
+        <v>1004</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>765</v>
+        <v>1005</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>766</v>
+        <v>1006</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>767</v>
+        <v>1007</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>768</v>
+        <v>1008</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>769</v>
+        <v>1009</v>
       </c>
       <c r="AY1" s="0" t="s">
-        <v>770</v>
+        <v>1010</v>
       </c>
       <c r="AZ1" s="0" t="s">
-        <v>771</v>
+        <v>1011</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>772</v>
+        <v>1012</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>773</v>
+        <v>1013</v>
       </c>
       <c r="BC1" s="0" t="s">
-        <v>774</v>
+        <v>1014</v>
       </c>
       <c r="BD1" s="0" t="s">
-        <v>775</v>
+        <v>1015</v>
       </c>
       <c r="BE1" s="0" t="s">
-        <v>776</v>
+        <v>1016</v>
       </c>
       <c r="BF1" s="0" t="s">
-        <v>777</v>
+        <v>1017</v>
       </c>
       <c r="BG1" s="0" t="s">
-        <v>778</v>
+        <v>1018</v>
       </c>
       <c r="BH1" s="0" t="s">
-        <v>779</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Added advanced plot for interpultion {i.e 4 times sample rate} Added work path dir to chosen ROI { e.g For F_1990 get the 3 corresponding ROI} Added ROI ONLY Plot
</commit_message>
<xml_diff>
--- a/Matlab_Main/Perfusion_data_Reg_MCA_LEFT.xlsx
+++ b/Matlab_Main/Perfusion_data_Reg_MCA_LEFT.xlsx
@@ -13,7 +13,187 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="1020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="1080">
+  <si>
+    <t>set1_1</t>
+  </si>
+  <si>
+    <t>set1_2</t>
+  </si>
+  <si>
+    <t>set2_1</t>
+  </si>
+  <si>
+    <t>set2_2</t>
+  </si>
+  <si>
+    <t>set3_1</t>
+  </si>
+  <si>
+    <t>set3_2</t>
+  </si>
+  <si>
+    <t>set4_1</t>
+  </si>
+  <si>
+    <t>set4_2</t>
+  </si>
+  <si>
+    <t>set5_1</t>
+  </si>
+  <si>
+    <t>set5_2</t>
+  </si>
+  <si>
+    <t>set6_1</t>
+  </si>
+  <si>
+    <t>set6_2</t>
+  </si>
+  <si>
+    <t>set7_1</t>
+  </si>
+  <si>
+    <t>set7_2</t>
+  </si>
+  <si>
+    <t>set8_1</t>
+  </si>
+  <si>
+    <t>set8_2</t>
+  </si>
+  <si>
+    <t>set9_1</t>
+  </si>
+  <si>
+    <t>set9_2</t>
+  </si>
+  <si>
+    <t>set10_1</t>
+  </si>
+  <si>
+    <t>set10_2</t>
+  </si>
+  <si>
+    <t>set11_1</t>
+  </si>
+  <si>
+    <t>set11_2</t>
+  </si>
+  <si>
+    <t>set12_1</t>
+  </si>
+  <si>
+    <t>set12_2</t>
+  </si>
+  <si>
+    <t>set13_1</t>
+  </si>
+  <si>
+    <t>set13_2</t>
+  </si>
+  <si>
+    <t>set14_1</t>
+  </si>
+  <si>
+    <t>set14_2</t>
+  </si>
+  <si>
+    <t>set15_1</t>
+  </si>
+  <si>
+    <t>set15_2</t>
+  </si>
+  <si>
+    <t>set16_1</t>
+  </si>
+  <si>
+    <t>set16_2</t>
+  </si>
+  <si>
+    <t>set17_1</t>
+  </si>
+  <si>
+    <t>set17_2</t>
+  </si>
+  <si>
+    <t>set18_1</t>
+  </si>
+  <si>
+    <t>set18_2</t>
+  </si>
+  <si>
+    <t>set19_1</t>
+  </si>
+  <si>
+    <t>set19_2</t>
+  </si>
+  <si>
+    <t>set20_1</t>
+  </si>
+  <si>
+    <t>set20_2</t>
+  </si>
+  <si>
+    <t>set21_1</t>
+  </si>
+  <si>
+    <t>set21_2</t>
+  </si>
+  <si>
+    <t>set22_1</t>
+  </si>
+  <si>
+    <t>set22_2</t>
+  </si>
+  <si>
+    <t>set23_1</t>
+  </si>
+  <si>
+    <t>set23_2</t>
+  </si>
+  <si>
+    <t>set24_1</t>
+  </si>
+  <si>
+    <t>set24_2</t>
+  </si>
+  <si>
+    <t>set25_1</t>
+  </si>
+  <si>
+    <t>set25_2</t>
+  </si>
+  <si>
+    <t>set26_1</t>
+  </si>
+  <si>
+    <t>set26_2</t>
+  </si>
+  <si>
+    <t>set27_1</t>
+  </si>
+  <si>
+    <t>set27_2</t>
+  </si>
+  <si>
+    <t>set28_1</t>
+  </si>
+  <si>
+    <t>set28_2</t>
+  </si>
+  <si>
+    <t>set29_1</t>
+  </si>
+  <si>
+    <t>set29_2</t>
+  </si>
+  <si>
+    <t>set30_1</t>
+  </si>
+  <si>
+    <t>set30_2</t>
+  </si>
   <si>
     <t>set1_1</t>
   </si>
@@ -3185,184 +3365,184 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>960</v>
+        <v>1020</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>961</v>
+        <v>1021</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>962</v>
+        <v>1022</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>963</v>
+        <v>1023</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>964</v>
+        <v>1024</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>965</v>
+        <v>1025</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>966</v>
+        <v>1026</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>967</v>
+        <v>1027</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>968</v>
+        <v>1028</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>969</v>
+        <v>1029</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>970</v>
+        <v>1030</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>971</v>
+        <v>1031</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>972</v>
+        <v>1032</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>973</v>
+        <v>1033</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>974</v>
+        <v>1034</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>975</v>
+        <v>1035</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>976</v>
+        <v>1036</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>977</v>
+        <v>1037</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>978</v>
+        <v>1038</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>979</v>
+        <v>1039</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>980</v>
+        <v>1040</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>981</v>
+        <v>1041</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>982</v>
+        <v>1042</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>983</v>
+        <v>1043</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>984</v>
+        <v>1044</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>985</v>
+        <v>1045</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>986</v>
+        <v>1046</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>987</v>
+        <v>1047</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>988</v>
+        <v>1048</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>989</v>
+        <v>1049</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>990</v>
+        <v>1050</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>991</v>
+        <v>1051</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>992</v>
+        <v>1052</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>993</v>
+        <v>1053</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>994</v>
+        <v>1054</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>995</v>
+        <v>1055</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>996</v>
+        <v>1056</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>997</v>
+        <v>1057</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>998</v>
+        <v>1058</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>999</v>
+        <v>1059</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>1000</v>
+        <v>1060</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>1001</v>
+        <v>1061</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>1002</v>
+        <v>1062</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>1003</v>
+        <v>1063</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>1004</v>
+        <v>1064</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>1006</v>
+        <v>1066</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>1007</v>
+        <v>1067</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>1008</v>
+        <v>1068</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>1009</v>
+        <v>1069</v>
       </c>
       <c r="AY1" s="0" t="s">
-        <v>1010</v>
+        <v>1070</v>
       </c>
       <c r="AZ1" s="0" t="s">
-        <v>1011</v>
+        <v>1071</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>1012</v>
+        <v>1072</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>1013</v>
+        <v>1073</v>
       </c>
       <c r="BC1" s="0" t="s">
-        <v>1014</v>
+        <v>1074</v>
       </c>
       <c r="BD1" s="0" t="s">
-        <v>1015</v>
+        <v>1075</v>
       </c>
       <c r="BE1" s="0" t="s">
-        <v>1016</v>
+        <v>1076</v>
       </c>
       <c r="BF1" s="0" t="s">
-        <v>1017</v>
+        <v>1077</v>
       </c>
       <c r="BG1" s="0" t="s">
-        <v>1018</v>
+        <v>1078</v>
       </c>
       <c r="BH1" s="0" t="s">
-        <v>1019</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="2">

</xml_diff>